<commit_message>
modified changes in the code
</commit_message>
<xml_diff>
--- a/data/TestExecution.xlsx
+++ b/data/TestExecution.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Sno</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>08</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -643,7 +640,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +718,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>11</v>
@@ -744,7 +741,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>11</v>
@@ -767,7 +764,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>11</v>
@@ -790,7 +787,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>11</v>
@@ -813,7 +810,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>11</v>
@@ -836,7 +833,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>11</v>
@@ -859,7 +856,7 @@
         <v>36</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>11</v>

</xml_diff>